<commit_message>
I modified the OF of the multifleet code and changing some things in opcost.m, not done yet
</commit_message>
<xml_diff>
--- a/Trial.xlsx
+++ b/Trial.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aishah\Google Drive\Magister\Kuliah\Quarter 6\AE4423 Airline Planning and Optimization\CPLEX &amp; Matlab\CPLEX &amp; Matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Claudia/Documents/MSc-1/Q2/AE4423/Airline-Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9320" yWindow="2200" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>PDL</t>
   </si>
@@ -33,12 +37,6 @@
   </si>
   <si>
     <t>LIS</t>
-  </si>
-  <si>
-    <t>TER</t>
-  </si>
-  <si>
-    <t>YYZ</t>
   </si>
   <si>
     <t>BOS</t>
@@ -119,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -705,21 +703,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -732,7 +730,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -758,7 +756,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -771,7 +769,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -784,7 +782,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -797,7 +795,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -810,7 +808,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -822,13 +820,13 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -902,7 +900,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>975</v>
@@ -925,7 +923,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>4545</v>
@@ -948,7 +946,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16">
         <v>3888</v>
@@ -971,7 +969,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -983,13 +981,13 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1063,7 +1061,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>558</v>
@@ -1086,7 +1084,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>770</v>
@@ -1109,7 +1107,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B25">
         <v>713</v>
@@ -1135,18 +1133,18 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
         <v>12</v>
-      </c>
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <v>0.12</v>
@@ -1155,12 +1153,12 @@
         <v>0.11</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>0.8</v>
@@ -1169,12 +1167,12 @@
         <v>0.8</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>240</v>
@@ -1183,12 +1181,12 @@
         <v>160</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B32">
         <v>9600</v>
@@ -1197,12 +1195,12 @@
         <v>5400</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B33">
         <v>900</v>
@@ -1211,12 +1209,12 @@
         <v>870</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>20</v>
@@ -1225,12 +1223,12 @@
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B35">
         <v>14</v>
@@ -1239,12 +1237,12 @@
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1253,12 +1251,12 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B37">
         <v>0.16</v>
@@ -1270,10 +1268,17 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>